<commit_message>
mostly done with everything
</commit_message>
<xml_diff>
--- a/Excel/Excel.xlsx
+++ b/Excel/Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/audreymongillo/Desktop/College/CS Class Materials/a2-DataVis-5Ways/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0E28B5F6-00FE-FE4B-872F-8D591667293E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{43BC4241-2029-DB40-9F24-19C2368EFEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1780" windowWidth="28360" windowHeight="18380" activeTab="1"/>
+    <workbookView xWindow="3480" yWindow="500" windowWidth="28360" windowHeight="18380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -619,6 +619,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9543CE"/>
+      <color rgb="FF842ACF"/>
       <color rgb="FFEBF1F4"/>
       <color rgb="FFE6EAEC"/>
       <color rgb="FFE3E6E6"/>
@@ -627,8 +629,6 @@
       <color rgb="FFC065F1"/>
       <color rgb="FF9D52AA"/>
       <color rgb="FF0092A0"/>
-      <color rgb="FF2180A1"/>
-      <color rgb="FFED7D31"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2090,7 +2090,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="A74BE3">
+              <a:srgbClr val="9543CE">
                 <a:alpha val="80000"/>
               </a:srgbClr>
             </a:solidFill>
@@ -24403,7 +24403,7 @@
   <dimension ref="A1:N152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E131" zoomScale="163" workbookViewId="0">
-      <selection activeCell="O139" sqref="O139"/>
+      <selection activeCell="O146" sqref="O146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>